<commit_message>
Added new feature files, new test data files and new test cases for SMB End2End suite, updated existing scenarios, added new methods at CucumberTempoFixture.java
</commit_message>
<xml_diff>
--- a/cucumber-for-appian/src/test/resources/testdata/02_SMB_End2End.xlsx
+++ b/cucumber-for-appian/src/test/resources/testdata/02_SMB_End2End.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\IdeaProjects\ORIXAutoExcel\cucumber-for-appian\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48218D18-C36F-49B5-BAEA-454EC7A01342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4DBB9D-BC1A-4075-A7F2-FD73E3FA91BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="873" xr2:uid="{25A2403C-A232-4567-AEA7-838C07E97658}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="873" xr2:uid="{25A2403C-A232-4567-AEA7-838C07E97658}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="13" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="198">
   <si>
     <t>Passenger cars including electric vehicles</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Entity Type</t>
   </si>
   <si>
-    <t>Do you want to use ORIX pricing?</t>
-  </si>
-  <si>
     <t>Is your quote from a Dealer?</t>
   </si>
   <si>
@@ -177,23 +174,6 @@
   </si>
   <si>
     <t>Engine Type</t>
-  </si>
-  <si>
-    <t>Fuel Type</t>
-  </si>
-  <si>
-    <t>Body Type</t>
-  </si>
-  <si>
-    <t>Drive Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Min Seats</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Max Seats</t>
   </si>
   <si>
     <t>Quote Document
@@ -224,9 +204,6 @@
   </si>
   <si>
     <t>Sole Trader</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>Select All Privacy Consent check boxes</t>
@@ -525,12 +502,6 @@
     <t>Company Name</t>
   </si>
   <si>
-    <t>Do you have a specific medium/heavy transport vehicle in mind?</t>
-  </si>
-  <si>
-    <t>Is the medium/heavy transport vehicle new?</t>
-  </si>
-  <si>
     <t>Vehicle or Asset Category</t>
   </si>
   <si>
@@ -579,13 +550,6 @@
     <t>27/05/1981</t>
   </si>
   <si>
-    <t>APP-545</t>
-  </si>
-  <si>
-    <t>SMB-00000785
-SMB-00000785</t>
-  </si>
-  <si>
     <t>Processing</t>
   </si>
   <si>
@@ -674,13 +638,32 @@
   </si>
   <si>
     <t>D:\ORIX_AUS\UploadDocs\Quote_Document.pdf</t>
+  </si>
+  <si>
+    <t>$0.00</t>
+  </si>
+  <si>
+    <t>$110,483.50</t>
+  </si>
+  <si>
+    <t>$4,597.98</t>
+  </si>
+  <si>
+    <t>APP-606</t>
+  </si>
+  <si>
+    <t>SMB-00000868
+SMB-00000868</t>
+  </si>
+  <si>
+    <t>02 Feb 2026 07:29 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -714,13 +697,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Univers"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos"/>
       <family val="2"/>
     </font>
     <font>
@@ -784,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -813,13 +789,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1156,13 +1129,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6282027D-BEC0-4DD3-B183-0B5114D5717E}">
-  <dimension ref="A1:DU22"/>
+  <dimension ref="A1:DM22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="CK2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CP2" sqref="CP2"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1174,81 +1147,80 @@
     <col min="5" max="5" width="7" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
     <col min="7" max="7" width="12.77734375" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" customWidth="1"/>
-    <col min="9" max="10" width="9.77734375" customWidth="1"/>
-    <col min="11" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" customWidth="1"/>
-    <col min="15" max="15" width="10.77734375" customWidth="1"/>
-    <col min="16" max="16" width="10.88671875" customWidth="1"/>
-    <col min="17" max="17" width="14.5546875" customWidth="1"/>
-    <col min="18" max="20" width="11.88671875" customWidth="1"/>
-    <col min="21" max="21" width="14.88671875" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" customWidth="1"/>
-    <col min="24" max="24" width="9.109375" customWidth="1"/>
-    <col min="25" max="25" width="11" customWidth="1"/>
-    <col min="26" max="26" width="8.88671875" customWidth="1"/>
-    <col min="27" max="27" width="8.6640625" customWidth="1"/>
-    <col min="28" max="35" width="6.5546875" customWidth="1"/>
-    <col min="37" max="37" width="8.5546875" customWidth="1"/>
-    <col min="38" max="41" width="8.44140625" customWidth="1"/>
-    <col min="43" max="43" width="6.33203125" customWidth="1"/>
-    <col min="44" max="44" width="14.5546875" customWidth="1"/>
-    <col min="45" max="45" width="6.88671875" customWidth="1"/>
-    <col min="46" max="46" width="5.77734375" customWidth="1"/>
-    <col min="47" max="47" width="4.33203125" customWidth="1"/>
-    <col min="48" max="48" width="4.44140625" customWidth="1"/>
-    <col min="49" max="49" width="4.77734375" customWidth="1"/>
-    <col min="50" max="50" width="4.88671875" customWidth="1"/>
-    <col min="51" max="51" width="5.21875" customWidth="1"/>
-    <col min="52" max="52" width="9.6640625" customWidth="1"/>
-    <col min="53" max="53" width="9.88671875" customWidth="1"/>
-    <col min="54" max="54" width="8.44140625" customWidth="1"/>
-    <col min="55" max="57" width="12.109375" customWidth="1"/>
-    <col min="58" max="58" width="13.6640625" customWidth="1"/>
-    <col min="59" max="59" width="15.33203125" customWidth="1"/>
-    <col min="60" max="61" width="21.33203125" customWidth="1"/>
-    <col min="62" max="62" width="15.88671875" customWidth="1"/>
-    <col min="63" max="63" width="21.44140625" customWidth="1"/>
-    <col min="64" max="64" width="18.6640625" customWidth="1"/>
-    <col min="65" max="65" width="18.33203125" customWidth="1"/>
-    <col min="66" max="66" width="19.109375" customWidth="1"/>
-    <col min="67" max="67" width="7.21875" customWidth="1"/>
-    <col min="68" max="68" width="7.77734375" customWidth="1"/>
-    <col min="69" max="69" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" customWidth="1"/>
+    <col min="11" max="11" width="17.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.77734375" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" customWidth="1"/>
+    <col min="15" max="17" width="6.21875" customWidth="1"/>
+    <col min="18" max="18" width="14.88671875" customWidth="1"/>
+    <col min="19" max="19" width="8.33203125" customWidth="1"/>
+    <col min="20" max="20" width="9" customWidth="1"/>
+    <col min="21" max="21" width="9.109375" customWidth="1"/>
+    <col min="22" max="22" width="11" customWidth="1"/>
+    <col min="23" max="23" width="8.88671875" customWidth="1"/>
+    <col min="24" max="24" width="8.6640625" customWidth="1"/>
+    <col min="25" max="32" width="6.5546875" customWidth="1"/>
+    <col min="34" max="34" width="8.5546875" customWidth="1"/>
+    <col min="35" max="35" width="8.44140625" customWidth="1"/>
+    <col min="36" max="36" width="7.21875" customWidth="1"/>
+    <col min="37" max="37" width="10" customWidth="1"/>
+    <col min="38" max="38" width="10.109375" customWidth="1"/>
+    <col min="40" max="40" width="6.33203125" customWidth="1"/>
+    <col min="41" max="41" width="14.5546875" customWidth="1"/>
+    <col min="42" max="42" width="6.88671875" customWidth="1"/>
+    <col min="43" max="43" width="5.77734375" customWidth="1"/>
+    <col min="44" max="44" width="7.33203125" customWidth="1"/>
+    <col min="45" max="45" width="9.88671875" customWidth="1"/>
+    <col min="46" max="46" width="8.44140625" customWidth="1"/>
+    <col min="47" max="49" width="12.109375" customWidth="1"/>
+    <col min="50" max="50" width="13.6640625" customWidth="1"/>
+    <col min="51" max="51" width="15.33203125" customWidth="1"/>
+    <col min="52" max="52" width="21.33203125" customWidth="1"/>
+    <col min="53" max="53" width="13.109375" customWidth="1"/>
+    <col min="54" max="54" width="15.88671875" customWidth="1"/>
+    <col min="55" max="55" width="21.44140625" customWidth="1"/>
+    <col min="56" max="56" width="18.6640625" customWidth="1"/>
+    <col min="57" max="57" width="18.33203125" customWidth="1"/>
+    <col min="58" max="58" width="19.109375" customWidth="1"/>
+    <col min="59" max="59" width="7.21875" customWidth="1"/>
+    <col min="60" max="60" width="7.77734375" customWidth="1"/>
+    <col min="61" max="61" width="12.6640625" customWidth="1"/>
+    <col min="62" max="62" width="10.109375" customWidth="1"/>
+    <col min="63" max="63" width="11.88671875" customWidth="1"/>
+    <col min="64" max="64" width="7.6640625" customWidth="1"/>
+    <col min="65" max="65" width="10.33203125" customWidth="1"/>
+    <col min="66" max="66" width="10.109375" customWidth="1"/>
+    <col min="67" max="67" width="12" customWidth="1"/>
+    <col min="68" max="68" width="12.109375" customWidth="1"/>
+    <col min="69" max="69" width="8.6640625" customWidth="1"/>
     <col min="70" max="70" width="10.109375" customWidth="1"/>
-    <col min="71" max="71" width="11.88671875" customWidth="1"/>
-    <col min="72" max="72" width="7.6640625" customWidth="1"/>
-    <col min="73" max="73" width="10.33203125" customWidth="1"/>
+    <col min="71" max="71" width="9.21875" customWidth="1"/>
+    <col min="72" max="72" width="12.109375" customWidth="1"/>
+    <col min="73" max="73" width="13.5546875" customWidth="1"/>
     <col min="74" max="74" width="10.109375" customWidth="1"/>
-    <col min="75" max="75" width="12" customWidth="1"/>
-    <col min="76" max="76" width="12.109375" customWidth="1"/>
-    <col min="77" max="77" width="8.6640625" customWidth="1"/>
-    <col min="78" max="78" width="10.109375" customWidth="1"/>
-    <col min="79" max="79" width="9.21875" customWidth="1"/>
-    <col min="80" max="80" width="12.109375" customWidth="1"/>
-    <col min="81" max="81" width="13.5546875" customWidth="1"/>
-    <col min="82" max="82" width="10.109375" customWidth="1"/>
-    <col min="83" max="84" width="23.109375" customWidth="1"/>
-    <col min="85" max="85" width="7.44140625" customWidth="1"/>
-    <col min="86" max="86" width="10.33203125" customWidth="1"/>
-    <col min="87" max="87" width="8.5546875" customWidth="1"/>
-    <col min="88" max="88" width="9.6640625" customWidth="1"/>
-    <col min="89" max="89" width="13.6640625" customWidth="1"/>
-    <col min="90" max="90" width="11.109375" customWidth="1"/>
-    <col min="91" max="91" width="14.6640625" customWidth="1"/>
-    <col min="92" max="92" width="28.44140625" customWidth="1"/>
-    <col min="93" max="93" width="17.77734375" customWidth="1"/>
-    <col min="94" max="94" width="14.6640625" customWidth="1"/>
-    <col min="95" max="95" width="19.77734375" customWidth="1"/>
-    <col min="96" max="124" width="14.6640625" customWidth="1"/>
-    <col min="125" max="125" width="27" customWidth="1"/>
+    <col min="75" max="75" width="23.109375" customWidth="1"/>
+    <col min="76" max="76" width="10.88671875" customWidth="1"/>
+    <col min="77" max="77" width="7.44140625" customWidth="1"/>
+    <col min="78" max="78" width="10.33203125" customWidth="1"/>
+    <col min="79" max="79" width="8.5546875" customWidth="1"/>
+    <col min="80" max="80" width="9.6640625" customWidth="1"/>
+    <col min="81" max="81" width="13.6640625" customWidth="1"/>
+    <col min="82" max="82" width="11.109375" customWidth="1"/>
+    <col min="83" max="83" width="14.6640625" customWidth="1"/>
+    <col min="84" max="84" width="28.44140625" customWidth="1"/>
+    <col min="85" max="85" width="9.77734375" customWidth="1"/>
+    <col min="86" max="86" width="14.6640625" customWidth="1"/>
+    <col min="87" max="87" width="19.77734375" customWidth="1"/>
+    <col min="88" max="116" width="14.6640625" customWidth="1"/>
+    <col min="117" max="117" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:125" s="3" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:117" s="3" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>39</v>
@@ -1263,313 +1235,313 @@
         <v>41</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AX1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="BK1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="BL1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BM1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="BN1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="BO1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="BP1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="BQ1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="BR1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="BS1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="BT1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="BU1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="BV1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="BW1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="BX1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="BY1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BZ1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="CA1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="CB1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="CC1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="CD1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="CE1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="CF1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="CG1" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" s="2" t="s">
+      <c r="CH1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="CI1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="AB1" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="AC1" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="AD1" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="AE1" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="AF1" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="AG1" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="AH1" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="AI1" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="AN1" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="AO1" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AZ1" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="BD1" s="2" t="s">
+      <c r="CJ1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="CK1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="CL1" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="CM1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="BF1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="BG1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="BH1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BI1" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="BJ1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="BK1" s="2" t="s">
+      <c r="CN1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="CO1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="BL1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="BM1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="BN1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="BO1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="BP1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BQ1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="BR1" s="2" t="s">
+      <c r="CP1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="BS1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="BT1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BU1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="BV1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="BW1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="BX1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="BY1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="BZ1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="CA1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="CB1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="CC1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="CD1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="CE1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="CF1" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="CG1" s="2" t="s">
+      <c r="CQ1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="CH1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="CI1" s="2" t="s">
+      <c r="CR1" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="CJ1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="CK1" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="CL1" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="CM1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="CN1" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="CO1" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="CP1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="CQ1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="CR1" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="CS1" s="2" t="s">
         <v>114</v>
       </c>
       <c r="CT1" s="2" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
       <c r="CU1" s="2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="CV1" s="2" t="s">
-        <v>107</v>
+        <v>157</v>
       </c>
       <c r="CW1" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="CX1" s="2" t="s">
         <v>117</v>
       </c>
       <c r="CY1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="CZ1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="DA1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="CZ1" s="2" t="s">
+      <c r="DB1" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="DA1" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="DB1" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="DC1" s="2" t="s">
         <v>122</v>
       </c>
       <c r="DD1" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="DE1" s="2" t="s">
         <v>123</v>
@@ -1578,66 +1550,42 @@
         <v>124</v>
       </c>
       <c r="DG1" s="2" t="s">
-        <v>33</v>
+        <v>125</v>
       </c>
       <c r="DH1" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="DI1" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="DJ1" s="2" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="DK1" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="DL1" s="2" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="DM1" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="DN1" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="DO1" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="DP1" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="DQ1" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="DR1" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="DS1" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="DT1" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="DU1" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:125" s="5" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:117" s="5" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C2" s="4">
         <v>39008846636</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>34</v>
@@ -1645,222 +1593,220 @@
       <c r="G2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="I2" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="K2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="4">
+      <c r="V2" s="4">
         <v>5</v>
       </c>
-      <c r="Z2" s="4">
+      <c r="W2" s="4">
         <v>0</v>
       </c>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
       <c r="AC2" s="4"/>
       <c r="AD2" s="4"/>
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
-      <c r="AG2" s="4"/>
-      <c r="AH2" s="4"/>
-      <c r="AI2" s="4"/>
-      <c r="AJ2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP2" s="4">
+        <v>2011</v>
+      </c>
+      <c r="AQ2" s="4"/>
+      <c r="AR2" s="4"/>
+      <c r="AS2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX2" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AY2" s="4">
+        <v>39008846636</v>
+      </c>
+      <c r="AZ2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AK2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" s="4" t="s">
+      <c r="BA2" s="4"/>
+      <c r="BB2" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AM2" s="4"/>
-      <c r="AN2" s="4"/>
-      <c r="AO2" s="4"/>
-      <c r="AP2" s="4" t="s">
+      <c r="BC2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="BD2" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="BE2" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AS2" s="4">
-        <v>2011</v>
-      </c>
-      <c r="AT2" s="4"/>
-      <c r="AU2" s="4"/>
-      <c r="AV2" s="4"/>
-      <c r="AW2" s="4"/>
-      <c r="AX2" s="4"/>
-      <c r="AY2" s="4"/>
-      <c r="AZ2" s="4"/>
-      <c r="BA2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BF2" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BC2" s="4" t="s">
+      <c r="BG2" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="BD2" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="BE2" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="BG2" s="4">
-        <v>39008846636</v>
       </c>
       <c r="BH2" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BI2" s="4"/>
+      <c r="BI2" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="BJ2" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="BK2" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="BK2" s="8" t="s">
+        <v>161</v>
+      </c>
       <c r="BL2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="BM2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="BN2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="BO2" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BM2" s="4" t="s">
+      <c r="BR2" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="BS2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BN2" s="4" t="s">
+      <c r="BT2" s="4">
+        <v>13501975</v>
+      </c>
+      <c r="BU2" s="4"/>
+      <c r="BV2" s="4"/>
+      <c r="BW2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BO2" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="BP2" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="BQ2" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="BR2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="BS2" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="BT2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="BU2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="BV2" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="BW2" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="BX2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BY2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="BZ2" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="CA2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="CB2" s="4">
-        <v>13501975</v>
-      </c>
+      <c r="BX2" s="4"/>
+      <c r="BY2" s="4"/>
+      <c r="BZ2" s="4"/>
+      <c r="CA2" s="4"/>
+      <c r="CB2" s="4"/>
       <c r="CC2" s="4"/>
       <c r="CD2" s="4"/>
       <c r="CE2" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="CF2" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="CF2" s="4" t="s">
+        <v>84</v>
+      </c>
       <c r="CG2" s="4"/>
-      <c r="CH2" s="4"/>
-      <c r="CI2" s="4"/>
-      <c r="CJ2" s="4"/>
-      <c r="CK2" s="4"/>
-      <c r="CL2" s="4"/>
+      <c r="CH2" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="CI2" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="CJ2" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="CK2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="CL2" s="4" t="s">
+        <v>162</v>
+      </c>
       <c r="CM2" s="4" t="s">
-        <v>62</v>
+        <v>197</v>
       </c>
       <c r="CN2" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="CO2" s="4"/>
+        <v>164</v>
+      </c>
+      <c r="CO2" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="CP2" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="CQ2" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="CR2" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="CQ2" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="CS2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="CT2" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="CU2" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="CV2" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="CW2" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="CX2" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="CY2" s="8" t="s">
-        <v>183</v>
-      </c>
+      <c r="CR2" s="8"/>
+      <c r="CS2" s="8"/>
+      <c r="CT2" s="8"/>
+      <c r="CU2" s="8"/>
+      <c r="CV2" s="8"/>
+      <c r="CW2" s="8"/>
+      <c r="CX2" s="8"/>
+      <c r="CY2" s="8"/>
       <c r="CZ2" s="8"/>
       <c r="DA2" s="8"/>
       <c r="DB2" s="8"/>
@@ -1874,33 +1820,25 @@
       <c r="DJ2" s="8"/>
       <c r="DK2" s="8"/>
       <c r="DL2" s="8"/>
-      <c r="DM2" s="8"/>
-      <c r="DN2" s="8"/>
-      <c r="DO2" s="8"/>
-      <c r="DP2" s="8"/>
-      <c r="DQ2" s="8"/>
-      <c r="DR2" s="8"/>
-      <c r="DS2" s="8"/>
-      <c r="DT2" s="8"/>
-      <c r="DU2" s="4" t="s">
-        <v>63</v>
+      <c r="DM2" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:125" s="5" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:117" s="5" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C3" s="4">
         <v>39008846636</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>34</v>
@@ -1908,286 +1846,278 @@
       <c r="G3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="I3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="K3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L3" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N3" s="4" t="s">
+      <c r="T3" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="4">
+        <v>5</v>
+      </c>
+      <c r="W3" s="4">
         <v>0</v>
       </c>
-      <c r="O3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="V3" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y3" s="4">
-        <v>5</v>
-      </c>
-      <c r="Z3" s="4">
-        <v>0</v>
-      </c>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
+      <c r="Z3" s="4"/>
       <c r="AA3" s="4"/>
       <c r="AB3" s="4"/>
       <c r="AC3" s="4"/>
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
       <c r="AF3" s="4"/>
-      <c r="AG3" s="4"/>
-      <c r="AH3" s="4"/>
-      <c r="AI3" s="4"/>
-      <c r="AJ3" s="4" t="s">
+      <c r="AG3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI3" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ3" s="4"/>
+      <c r="AK3" s="4"/>
+      <c r="AL3" s="4"/>
+      <c r="AM3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP3" s="4">
+        <v>2011</v>
+      </c>
+      <c r="AQ3" s="4"/>
+      <c r="AR3" s="4"/>
+      <c r="AS3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW3" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AY3" s="4">
+        <v>39008846636</v>
+      </c>
+      <c r="AZ3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AK3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL3" s="4" t="s">
+      <c r="BA3" s="4"/>
+      <c r="BB3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AM3" s="4"/>
-      <c r="AN3" s="4"/>
-      <c r="AO3" s="4"/>
-      <c r="AP3" s="4" t="s">
+      <c r="BC3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AQ3" s="4" t="s">
+      <c r="BD3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AR3" s="4" t="s">
+      <c r="BE3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AS3" s="4">
-        <v>2011</v>
-      </c>
-      <c r="AT3" s="4"/>
-      <c r="AU3" s="4"/>
-      <c r="AV3" s="4"/>
-      <c r="AW3" s="4"/>
-      <c r="AX3" s="4"/>
-      <c r="AY3" s="4"/>
-      <c r="AZ3" s="4"/>
-      <c r="BA3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="BB3" s="4" t="s">
+      <c r="BF3" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BC3" s="4" t="s">
+      <c r="BG3" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="BD3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="BE3" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF3" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="BG3" s="4">
-        <v>39008846636</v>
       </c>
       <c r="BH3" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BI3" s="4"/>
+      <c r="BI3" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="BJ3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="BK3" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="BK3" s="8" t="s">
+        <v>161</v>
+      </c>
       <c r="BL3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="BM3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="BN3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="BO3" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="BP3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="BQ3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BM3" s="4" t="s">
+      <c r="BR3" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="BS3" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BN3" s="4" t="s">
+      <c r="BT3" s="4">
+        <v>13501975</v>
+      </c>
+      <c r="BU3" s="4"/>
+      <c r="BV3" s="4"/>
+      <c r="BW3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BO3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="BP3" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="BQ3" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="BR3" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="BS3" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="BT3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="BU3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="BV3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="BW3" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="BX3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BY3" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="BZ3" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="CA3" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="CB3" s="4">
-        <v>13501975</v>
-      </c>
-      <c r="CC3" s="4"/>
+      <c r="BX3" s="4"/>
+      <c r="BY3" s="4"/>
+      <c r="BZ3" s="4"/>
+      <c r="CA3" s="4"/>
+      <c r="CB3" s="4"/>
+      <c r="CC3" s="4" t="s">
+        <v>171</v>
+      </c>
       <c r="CD3" s="4"/>
       <c r="CE3" s="4" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="CF3" s="4"/>
       <c r="CG3" s="4"/>
       <c r="CH3" s="4"/>
-      <c r="CI3" s="4"/>
-      <c r="CJ3" s="4"/>
+      <c r="CI3" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="CJ3" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="CK3" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="CL3" s="4"/>
+        <v>168</v>
+      </c>
+      <c r="CL3" s="4" t="s">
+        <v>170</v>
+      </c>
       <c r="CM3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="CN3" s="4"/>
-      <c r="CO3" s="4"/>
-      <c r="CP3" s="4"/>
-      <c r="CQ3" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="CN3" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="CO3" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="CP3" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="CQ3" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="CR3" s="8"/>
+      <c r="CS3" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="CT3" s="8"/>
+      <c r="CU3" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="CV3" s="8"/>
+      <c r="CW3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="CX3" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="CY3" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="CZ3" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="CR3" s="4" t="s">
+      <c r="DA3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="DB3" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="CS3" s="4" t="s">
+      <c r="DC3" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="CT3" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="CU3" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="CV3" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="CW3" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="CX3" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="CY3" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="CZ3" s="8"/>
-      <c r="DA3" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="DB3" s="8"/>
-      <c r="DC3" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="DD3" s="8"/>
       <c r="DE3" s="8" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="DF3" s="8" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="DG3" s="8" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="DH3" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="DI3" s="8"/>
+      <c r="DJ3" s="8"/>
+      <c r="DK3" s="8"/>
+      <c r="DL3" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="DM3" s="4"/>
+    </row>
+    <row r="4" spans="1:117" s="5" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="DI3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="DJ3" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="DK3" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="DL3" s="8"/>
-      <c r="DM3" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="DN3" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="DO3" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="DP3" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="DQ3" s="8"/>
-      <c r="DR3" s="8"/>
-      <c r="DS3" s="8"/>
-      <c r="DT3" s="8" t="s">
-        <v>195</v>
-      </c>
-      <c r="DU3" s="4"/>
-    </row>
-    <row r="4" spans="1:125" s="5" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>199</v>
-      </c>
       <c r="B4" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C4" s="4">
         <v>39008846636</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>34</v>
@@ -2195,290 +2125,280 @@
       <c r="G4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="I4" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="K4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Y4" s="4">
+      <c r="V4" s="4">
         <v>5</v>
       </c>
-      <c r="Z4" s="4">
+      <c r="W4" s="4">
         <v>0</v>
       </c>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
+      <c r="Z4" s="4"/>
       <c r="AA4" s="4"/>
       <c r="AB4" s="4"/>
       <c r="AC4" s="4"/>
       <c r="AD4" s="4"/>
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
-      <c r="AJ4" s="4" t="s">
+      <c r="AG4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ4" s="4"/>
+      <c r="AK4" s="4"/>
+      <c r="AL4" s="4"/>
+      <c r="AM4" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO4" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP4" s="4">
+        <v>2011</v>
+      </c>
+      <c r="AQ4" s="4"/>
+      <c r="AR4" s="4"/>
+      <c r="AS4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV4" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AY4" s="4">
+        <v>39008846636</v>
+      </c>
+      <c r="AZ4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AK4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL4" s="4" t="s">
+      <c r="BA4" s="4"/>
+      <c r="BB4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
-      <c r="AO4" s="4"/>
-      <c r="AP4" s="4" t="s">
+      <c r="BC4" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AQ4" s="4" t="s">
+      <c r="BD4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AR4" s="4" t="s">
+      <c r="BE4" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AS4" s="4">
-        <v>2011</v>
-      </c>
-      <c r="AT4" s="4"/>
-      <c r="AU4" s="4"/>
-      <c r="AV4" s="4"/>
-      <c r="AW4" s="4"/>
-      <c r="AX4" s="4"/>
-      <c r="AY4" s="4"/>
-      <c r="AZ4" s="4"/>
-      <c r="BA4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="BB4" s="4" t="s">
+      <c r="BF4" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BC4" s="4" t="s">
+      <c r="BG4" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="BD4" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="BE4" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF4" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="BG4" s="4">
-        <v>39008846636</v>
       </c>
       <c r="BH4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BI4" s="4"/>
+      <c r="BI4" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="BJ4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="BK4" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="BK4" s="8" t="s">
+        <v>161</v>
+      </c>
       <c r="BL4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="BM4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="BN4" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="BO4" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="BP4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="BQ4" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BM4" s="4" t="s">
+      <c r="BR4" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="BS4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BN4" s="4" t="s">
+      <c r="BT4" s="4">
+        <v>13501975</v>
+      </c>
+      <c r="BU4" s="4"/>
+      <c r="BV4" s="4"/>
+      <c r="BW4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BO4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="BP4" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="BQ4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="BR4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="BS4" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="BT4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="BU4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="BV4" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="BW4" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="BX4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BY4" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="BZ4" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="CA4" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="CB4" s="4">
-        <v>13501975</v>
-      </c>
-      <c r="CC4" s="4"/>
+      <c r="BX4" s="4"/>
+      <c r="BY4" s="4"/>
+      <c r="BZ4" s="4"/>
+      <c r="CA4" s="4"/>
+      <c r="CB4" s="4"/>
+      <c r="CC4" s="4" t="s">
+        <v>171</v>
+      </c>
       <c r="CD4" s="4"/>
       <c r="CE4" s="4" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="CF4" s="4"/>
       <c r="CG4" s="4"/>
       <c r="CH4" s="4"/>
-      <c r="CI4" s="4"/>
-      <c r="CJ4" s="4"/>
+      <c r="CI4" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="CJ4" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="CK4" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="CL4" s="4"/>
+        <v>168</v>
+      </c>
+      <c r="CL4" s="4" t="s">
+        <v>170</v>
+      </c>
       <c r="CM4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="CN4" s="4"/>
-      <c r="CO4" s="4"/>
-      <c r="CP4" s="4"/>
-      <c r="CQ4" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="CN4" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="CO4" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="CP4" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="CQ4" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="CR4" s="8"/>
+      <c r="CS4" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="CT4" s="8"/>
+      <c r="CU4" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="CV4" s="8"/>
+      <c r="CW4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="CX4" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="CY4" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="CZ4" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="CR4" s="4" t="s">
+      <c r="DA4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="DB4" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="CS4" s="4" t="s">
+      <c r="DC4" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="CT4" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="CU4" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="CV4" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="CW4" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="CX4" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="CY4" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="CZ4" s="8"/>
-      <c r="DA4" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="DB4" s="8"/>
-      <c r="DC4" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="DD4" s="8"/>
       <c r="DE4" s="8" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="DF4" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="DG4" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="DH4" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="DI4" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="DG4" s="8" t="s">
+      <c r="DJ4" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="DH4" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="DI4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="DJ4" s="8" t="s">
+      <c r="DK4" s="8"/>
+      <c r="DL4" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="DM4" s="4"/>
+    </row>
+    <row r="5" spans="1:117" s="5" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="DK4" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="DL4" s="8"/>
-      <c r="DM4" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="DN4" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="DO4" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="DP4" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="DQ4" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="DR4" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="DS4" s="8"/>
-      <c r="DT4" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="DU4" s="4"/>
-    </row>
-    <row r="5" spans="1:125" s="5" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>200</v>
-      </c>
       <c r="B5" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C5" s="4">
         <v>39008846636</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F5" s="4" t="s">
         <v>34</v>
@@ -2486,276 +2406,266 @@
       <c r="G5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="I5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="K5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="S5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="V5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="Y5" s="4">
+      <c r="V5" s="4">
         <v>5</v>
       </c>
-      <c r="Z5" s="4">
+      <c r="W5" s="4">
         <v>0</v>
       </c>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
       <c r="AC5" s="4"/>
       <c r="AD5" s="4"/>
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
-      <c r="AG5" s="4"/>
-      <c r="AH5" s="4"/>
-      <c r="AI5" s="4"/>
-      <c r="AJ5" s="4" t="s">
+      <c r="AG5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ5" s="4"/>
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4"/>
+      <c r="AM5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP5" s="4">
+        <v>2011</v>
+      </c>
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4"/>
+      <c r="AS5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AV5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AW5" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AY5" s="4">
+        <v>39008846636</v>
+      </c>
+      <c r="AZ5" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AK5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL5" s="4" t="s">
+      <c r="BA5" s="4"/>
+      <c r="BB5" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="4"/>
-      <c r="AO5" s="4"/>
-      <c r="AP5" s="4" t="s">
+      <c r="BC5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="AQ5" s="4" t="s">
+      <c r="BD5" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="AR5" s="4" t="s">
+      <c r="BE5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AS5" s="4">
-        <v>2011</v>
-      </c>
-      <c r="AT5" s="4"/>
-      <c r="AU5" s="4"/>
-      <c r="AV5" s="4"/>
-      <c r="AW5" s="4"/>
-      <c r="AX5" s="4"/>
-      <c r="AY5" s="4"/>
-      <c r="AZ5" s="4"/>
-      <c r="BA5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="BB5" s="4" t="s">
+      <c r="BF5" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="BC5" s="4" t="s">
+      <c r="BG5" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="BD5" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="BE5" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="BF5" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="BG5" s="4">
-        <v>39008846636</v>
       </c>
       <c r="BH5" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="BI5" s="4"/>
+      <c r="BI5" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="BJ5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="BK5" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="BK5" s="8" t="s">
+        <v>161</v>
+      </c>
       <c r="BL5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="BM5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="BN5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="BO5" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="BP5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="BQ5" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BM5" s="4" t="s">
+      <c r="BR5" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="BS5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BN5" s="4" t="s">
+      <c r="BT5" s="4">
+        <v>13501975</v>
+      </c>
+      <c r="BU5" s="4"/>
+      <c r="BV5" s="4"/>
+      <c r="BW5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BO5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="BP5" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="BQ5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="BR5" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="BS5" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="BT5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="BU5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="BV5" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="BW5" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="BX5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="BY5" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="BZ5" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="CA5" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="CB5" s="4">
-        <v>13501975</v>
-      </c>
-      <c r="CC5" s="4"/>
+      <c r="BX5" s="4"/>
+      <c r="BY5" s="4"/>
+      <c r="BZ5" s="4"/>
+      <c r="CA5" s="4"/>
+      <c r="CB5" s="4"/>
+      <c r="CC5" s="4" t="s">
+        <v>171</v>
+      </c>
       <c r="CD5" s="4"/>
       <c r="CE5" s="4" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="CF5" s="4"/>
       <c r="CG5" s="4"/>
       <c r="CH5" s="4"/>
-      <c r="CI5" s="4"/>
-      <c r="CJ5" s="4"/>
+      <c r="CI5" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="CJ5" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="CK5" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="CL5" s="4"/>
+        <v>168</v>
+      </c>
+      <c r="CL5" s="4" t="s">
+        <v>170</v>
+      </c>
       <c r="CM5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="CN5" s="4"/>
-      <c r="CO5" s="4"/>
-      <c r="CP5" s="4"/>
-      <c r="CQ5" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="CN5" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="CO5" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="CP5" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="CQ5" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="CR5" s="8"/>
+      <c r="CS5" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="CT5" s="8"/>
+      <c r="CU5" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="CV5" s="8"/>
+      <c r="CW5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="CX5" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="CY5" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="CZ5" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="CR5" s="4" t="s">
+      <c r="DA5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="DB5" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="CS5" s="4" t="s">
+      <c r="DC5" s="8" t="s">
         <v>179</v>
-      </c>
-      <c r="CT5" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="CU5" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="CV5" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="CW5" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="CX5" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="CY5" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="CZ5" s="8"/>
-      <c r="DA5" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="DB5" s="8"/>
-      <c r="DC5" s="8" t="s">
-        <v>185</v>
       </c>
       <c r="DD5" s="8"/>
       <c r="DE5" s="8" t="s">
-        <v>32</v>
+        <v>180</v>
       </c>
       <c r="DF5" s="8" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="DG5" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="DH5" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="DI5" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="DJ5" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="DH5" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="DI5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="DJ5" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="DK5" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="DL5" s="8"/>
-      <c r="DM5" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="DN5" s="8" t="s">
-        <v>192</v>
-      </c>
-      <c r="DO5" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="DP5" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="DQ5" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="DR5" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="DS5" s="8"/>
-      <c r="DT5" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="DU5" s="4"/>
+      <c r="DK5" s="8"/>
+      <c r="DL5" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="DM5" s="4"/>
     </row>
-    <row r="6" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -2873,16 +2783,8 @@
       <c r="DK6" s="6"/>
       <c r="DL6" s="6"/>
       <c r="DM6" s="6"/>
-      <c r="DN6" s="6"/>
-      <c r="DO6" s="6"/>
-      <c r="DP6" s="6"/>
-      <c r="DQ6" s="6"/>
-      <c r="DR6" s="6"/>
-      <c r="DS6" s="6"/>
-      <c r="DT6" s="6"/>
-      <c r="DU6" s="6"/>
     </row>
-    <row r="7" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -3000,16 +2902,8 @@
       <c r="DK7" s="6"/>
       <c r="DL7" s="6"/>
       <c r="DM7" s="6"/>
-      <c r="DN7" s="6"/>
-      <c r="DO7" s="6"/>
-      <c r="DP7" s="6"/>
-      <c r="DQ7" s="6"/>
-      <c r="DR7" s="6"/>
-      <c r="DS7" s="6"/>
-      <c r="DT7" s="6"/>
-      <c r="DU7" s="6"/>
     </row>
-    <row r="8" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
@@ -3127,16 +3021,8 @@
       <c r="DK8" s="6"/>
       <c r="DL8" s="6"/>
       <c r="DM8" s="6"/>
-      <c r="DN8" s="6"/>
-      <c r="DO8" s="6"/>
-      <c r="DP8" s="6"/>
-      <c r="DQ8" s="6"/>
-      <c r="DR8" s="6"/>
-      <c r="DS8" s="6"/>
-      <c r="DT8" s="6"/>
-      <c r="DU8" s="6"/>
     </row>
-    <row r="9" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -3254,16 +3140,8 @@
       <c r="DK9" s="6"/>
       <c r="DL9" s="6"/>
       <c r="DM9" s="6"/>
-      <c r="DN9" s="6"/>
-      <c r="DO9" s="6"/>
-      <c r="DP9" s="6"/>
-      <c r="DQ9" s="6"/>
-      <c r="DR9" s="6"/>
-      <c r="DS9" s="6"/>
-      <c r="DT9" s="6"/>
-      <c r="DU9" s="6"/>
     </row>
-    <row r="10" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -3381,16 +3259,8 @@
       <c r="DK10" s="6"/>
       <c r="DL10" s="6"/>
       <c r="DM10" s="6"/>
-      <c r="DN10" s="6"/>
-      <c r="DO10" s="6"/>
-      <c r="DP10" s="6"/>
-      <c r="DQ10" s="6"/>
-      <c r="DR10" s="6"/>
-      <c r="DS10" s="6"/>
-      <c r="DT10" s="6"/>
-      <c r="DU10" s="6"/>
     </row>
-    <row r="11" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -3508,16 +3378,8 @@
       <c r="DK11" s="6"/>
       <c r="DL11" s="6"/>
       <c r="DM11" s="6"/>
-      <c r="DN11" s="6"/>
-      <c r="DO11" s="6"/>
-      <c r="DP11" s="6"/>
-      <c r="DQ11" s="6"/>
-      <c r="DR11" s="6"/>
-      <c r="DS11" s="6"/>
-      <c r="DT11" s="6"/>
-      <c r="DU11" s="6"/>
     </row>
-    <row r="12" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
@@ -3635,16 +3497,8 @@
       <c r="DK12" s="6"/>
       <c r="DL12" s="6"/>
       <c r="DM12" s="6"/>
-      <c r="DN12" s="6"/>
-      <c r="DO12" s="6"/>
-      <c r="DP12" s="6"/>
-      <c r="DQ12" s="6"/>
-      <c r="DR12" s="6"/>
-      <c r="DS12" s="6"/>
-      <c r="DT12" s="6"/>
-      <c r="DU12" s="6"/>
     </row>
-    <row r="13" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -3762,16 +3616,8 @@
       <c r="DK13" s="6"/>
       <c r="DL13" s="6"/>
       <c r="DM13" s="6"/>
-      <c r="DN13" s="6"/>
-      <c r="DO13" s="6"/>
-      <c r="DP13" s="6"/>
-      <c r="DQ13" s="6"/>
-      <c r="DR13" s="6"/>
-      <c r="DS13" s="6"/>
-      <c r="DT13" s="6"/>
-      <c r="DU13" s="6"/>
     </row>
-    <row r="14" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -3889,16 +3735,8 @@
       <c r="DK14" s="6"/>
       <c r="DL14" s="6"/>
       <c r="DM14" s="6"/>
-      <c r="DN14" s="6"/>
-      <c r="DO14" s="6"/>
-      <c r="DP14" s="6"/>
-      <c r="DQ14" s="6"/>
-      <c r="DR14" s="6"/>
-      <c r="DS14" s="6"/>
-      <c r="DT14" s="6"/>
-      <c r="DU14" s="6"/>
     </row>
-    <row r="15" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -4016,16 +3854,8 @@
       <c r="DK15" s="6"/>
       <c r="DL15" s="6"/>
       <c r="DM15" s="6"/>
-      <c r="DN15" s="6"/>
-      <c r="DO15" s="6"/>
-      <c r="DP15" s="6"/>
-      <c r="DQ15" s="6"/>
-      <c r="DR15" s="6"/>
-      <c r="DS15" s="6"/>
-      <c r="DT15" s="6"/>
-      <c r="DU15" s="6"/>
     </row>
-    <row r="16" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
@@ -4143,16 +3973,8 @@
       <c r="DK16" s="6"/>
       <c r="DL16" s="6"/>
       <c r="DM16" s="6"/>
-      <c r="DN16" s="6"/>
-      <c r="DO16" s="6"/>
-      <c r="DP16" s="6"/>
-      <c r="DQ16" s="6"/>
-      <c r="DR16" s="6"/>
-      <c r="DS16" s="6"/>
-      <c r="DT16" s="6"/>
-      <c r="DU16" s="6"/>
     </row>
-    <row r="17" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -4270,16 +4092,8 @@
       <c r="DK17" s="6"/>
       <c r="DL17" s="6"/>
       <c r="DM17" s="6"/>
-      <c r="DN17" s="6"/>
-      <c r="DO17" s="6"/>
-      <c r="DP17" s="6"/>
-      <c r="DQ17" s="6"/>
-      <c r="DR17" s="6"/>
-      <c r="DS17" s="6"/>
-      <c r="DT17" s="6"/>
-      <c r="DU17" s="6"/>
     </row>
-    <row r="18" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -4397,16 +4211,8 @@
       <c r="DK18" s="6"/>
       <c r="DL18" s="6"/>
       <c r="DM18" s="6"/>
-      <c r="DN18" s="6"/>
-      <c r="DO18" s="6"/>
-      <c r="DP18" s="6"/>
-      <c r="DQ18" s="6"/>
-      <c r="DR18" s="6"/>
-      <c r="DS18" s="6"/>
-      <c r="DT18" s="6"/>
-      <c r="DU18" s="6"/>
     </row>
-    <row r="19" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
@@ -4524,16 +4330,8 @@
       <c r="DK19" s="6"/>
       <c r="DL19" s="6"/>
       <c r="DM19" s="6"/>
-      <c r="DN19" s="6"/>
-      <c r="DO19" s="6"/>
-      <c r="DP19" s="6"/>
-      <c r="DQ19" s="6"/>
-      <c r="DR19" s="6"/>
-      <c r="DS19" s="6"/>
-      <c r="DT19" s="6"/>
-      <c r="DU19" s="6"/>
     </row>
-    <row r="20" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
@@ -4651,16 +4449,8 @@
       <c r="DK20" s="6"/>
       <c r="DL20" s="6"/>
       <c r="DM20" s="6"/>
-      <c r="DN20" s="6"/>
-      <c r="DO20" s="6"/>
-      <c r="DP20" s="6"/>
-      <c r="DQ20" s="6"/>
-      <c r="DR20" s="6"/>
-      <c r="DS20" s="6"/>
-      <c r="DT20" s="6"/>
-      <c r="DU20" s="6"/>
     </row>
-    <row r="21" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -4778,16 +4568,8 @@
       <c r="DK21" s="6"/>
       <c r="DL21" s="6"/>
       <c r="DM21" s="6"/>
-      <c r="DN21" s="6"/>
-      <c r="DO21" s="6"/>
-      <c r="DP21" s="6"/>
-      <c r="DQ21" s="6"/>
-      <c r="DR21" s="6"/>
-      <c r="DS21" s="6"/>
-      <c r="DT21" s="6"/>
-      <c r="DU21" s="6"/>
     </row>
-    <row r="22" spans="1:125" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:117" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -4905,21 +4687,13 @@
       <c r="DK22" s="6"/>
       <c r="DL22" s="6"/>
       <c r="DM22" s="6"/>
-      <c r="DN22" s="6"/>
-      <c r="DO22" s="6"/>
-      <c r="DP22" s="6"/>
-      <c r="DQ22" s="6"/>
-      <c r="DR22" s="6"/>
-      <c r="DS22" s="6"/>
-      <c r="DT22" s="6"/>
-      <c r="DU22" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BX2" r:id="rId1" xr:uid="{5A65F2F1-85B7-4BDE-914B-E5E798F153DB}"/>
-    <hyperlink ref="BX3" r:id="rId2" xr:uid="{77A0ABB5-F598-450A-9606-1453386A8216}"/>
-    <hyperlink ref="BX4" r:id="rId3" xr:uid="{9C79A9B2-F3E6-4A88-BA65-FA98965FC531}"/>
-    <hyperlink ref="BX5" r:id="rId4" xr:uid="{A368E10F-1FD3-43FF-8900-02A2FEA4C7D5}"/>
+    <hyperlink ref="BP2" r:id="rId1" xr:uid="{5A65F2F1-85B7-4BDE-914B-E5E798F153DB}"/>
+    <hyperlink ref="BP3" r:id="rId2" xr:uid="{77A0ABB5-F598-450A-9606-1453386A8216}"/>
+    <hyperlink ref="BP4" r:id="rId3" xr:uid="{9C79A9B2-F3E6-4A88-BA65-FA98965FC531}"/>
+    <hyperlink ref="BP5" r:id="rId4" xr:uid="{A368E10F-1FD3-43FF-8900-02A2FEA4C7D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>